<commit_message>
Tratamento de erros preliminar construído
Tratamento de erros baseado no modo pânico.
</commit_message>
<xml_diff>
--- a/TabelaSintatica/TabelaSintatica.xlsx
+++ b/TabelaSintatica/TabelaSintatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Compiladores20201\CompiladorALGOL\TabelaSintatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9B1F8A-ABB9-4145-A4DA-676EACA245CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99420AB8-1D8D-4846-9CEE-0AF81540D99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="380" xr2:uid="{F6ACE99F-4ECF-4226-A515-6C36F058829F}"/>
   </bookViews>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3068961D-FDE1-4255-837F-16A5070B835C}">
   <dimension ref="A1:AM61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>